<commit_message>
3rd Chamber Sensor Test
</commit_message>
<xml_diff>
--- a/Testing/Ash Chamber Sensor Testing/Testing 16 Aug/DSL-460 MkII 2016-08-16 Filtered Data.xlsx
+++ b/Testing/Ash Chamber Sensor Testing/Testing 16 Aug/DSL-460 MkII 2016-08-16 Filtered Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\Testing\Ash Chamber Sensor Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\Testing\Ash Chamber Sensor Testing\Testing 16 Aug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DSL-460 MkII SN10006 ReadingsFi'!$I$1:$I$2364</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -861,8 +861,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I2364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="B350" workbookViewId="0">
+      <selection activeCell="M694" sqref="M694"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>